<commit_message>
update register from login page
</commit_message>
<xml_diff>
--- a/LambdaTest_Playwright_Java/src/test/resources/TestCases/LambdaTest_Ecommerce Test Cases.xlsx
+++ b/LambdaTest_Playwright_Java/src/test/resources/TestCases/LambdaTest_Ecommerce Test Cases.xlsx
@@ -4,21 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="360" windowWidth="18820" windowHeight="7060" activeTab="3"/>
+    <workbookView xWindow="320" yWindow="360" windowWidth="18820" windowHeight="7060" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TC01_Login" sheetId="1" r:id="rId1"/>
     <sheet name="TC02_RegisterUser" sheetId="3" r:id="rId2"/>
     <sheet name="TC03_ForgotPassword" sheetId="2" r:id="rId3"/>
-    <sheet name="TC04_MyAccount" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="5" r:id="rId5"/>
+    <sheet name="TC05_MyAccount" sheetId="4" r:id="rId4"/>
+    <sheet name="TC04_RegisterFromLoginPage" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="103">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -289,42 +289,6 @@
     <t>Verify email input with unregistered/invalid email</t>
   </si>
   <si>
-    <t>Test Case ID | Test Scenario                               | Steps to Execute                                                                 | Expected Result                              | Actual Result | Pass/Fail |</t>
-  </si>
-  <si>
-    <t>-------------|---------------------------------------------|----------------------------------------------------------------------------------|----------------------------------------------|---------------|-----------|</t>
-  </si>
-  <si>
-    <t>TC001        | Access My Account Page                      | 1. Log in to the application \n2. Navigate to the "My Account" page               | "My Account" page loads successfully          |               |           |</t>
-  </si>
-  <si>
-    <t>TC002        | Update Profile Information                  | 1. Log in to the application \n2. Navigate to "My Account" page \n3. Update profile info \n4. Save changes | Profile info updated successfully            |               |           |</t>
-  </si>
-  <si>
-    <t>TC003        | Invalid Profile Information                 | 1. Log in to the application \n2. Navigate to "My Account" page \n3. Enter invalid profile info \n4. Save changes | Error message displayed                      |               |           |</t>
-  </si>
-  <si>
-    <t>TC004        | Leave Required Fields Empty                 | 1. Log in to the application \n2. Navigate to "My Account" page \n3. Leave required fields empty \n4. Save changes | Validation messages displayed                 |               |           |</t>
-  </si>
-  <si>
-    <t>TC005        | Change Password with Valid Data             | 1. Log in to the application \n2. Navigate to "My Account" page \n3. Change password with valid data \n4. Save changes | Password changed successfully                 |               |           |</t>
-  </si>
-  <si>
-    <t>TC006        | Change Password with Invalid Data           | 1. Log in to the application \n2. Navigate to "My Account" page \n3. Change password with invalid data \n4. Save changes | Error message displayed                       |               |           |</t>
-  </si>
-  <si>
-    <t>TC007        | Check Order History                         | 1. Log in to the application \n2. Navigate to "My Account" page \n3. View order history | Order history displayed correctly             |               |           |</t>
-  </si>
-  <si>
-    <t>TC008        | Check Order History with No Orders          | 1. Log in to the application \n2. Navigate to "My Account" page \n3. View order history | "No orders found" message displayed          |               |           |</t>
-  </si>
-  <si>
-    <t>TC009        | Logout from My Account Page                 | 1. Log in to the application \n2. Navigate to "My Account" page \n3. Click "Logout" button | User logged out and redirected to login page |               |           |</t>
-  </si>
-  <si>
-    <t>TC010        | Access My Account Page Without Login        | 1. Navigate to "My Account" page without logging in                              | Redirected to login page                      |               |           |</t>
-  </si>
-  <si>
     <t>Verify user is able to Access My Account Page</t>
   </si>
   <si>
@@ -404,6 +368,27 @@
   </si>
   <si>
     <t>Login page loads successfully</t>
+  </si>
+  <si>
+    <t>TC01</t>
+  </si>
+  <si>
+    <t>Verify Register Link/Icon is visible on login page</t>
+  </si>
+  <si>
+    <t>The Register link should be present on the login page.</t>
+  </si>
+  <si>
+    <t>TC02</t>
+  </si>
+  <si>
+    <t>Verify user is able to navigate to register page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Launch the application.                       2. Navigate to the login screen            3. Click on Register Link </t>
+  </si>
+  <si>
+    <t>User should be navigated to the Register page.</t>
   </si>
 </sst>
 </file>
@@ -480,14 +465,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -961,7 +946,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1137,7 +1122,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1268,21 +1253,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:F9"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.54296875" style="6" customWidth="1"/>
-    <col min="2" max="2" width="23.54296875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="18.26953125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="35.81640625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="26.36328125" style="6" customWidth="1"/>
-    <col min="6" max="6" width="16.08984375" style="6" customWidth="1"/>
-    <col min="7" max="7" width="8.7265625" style="6"/>
-    <col min="8" max="8" width="12.54296875" style="6" customWidth="1"/>
-    <col min="9" max="16384" width="8.7265625" style="6"/>
+    <col min="1" max="1" width="13.54296875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="23.54296875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="18.26953125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="35.81640625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="26.36328125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="16.08984375" style="5" customWidth="1"/>
+    <col min="7" max="7" width="8.7265625" style="5"/>
+    <col min="8" max="8" width="12.54296875" style="5" customWidth="1"/>
+    <col min="9" max="16384" width="8.7265625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -1312,180 +1297,180 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>81</v>
+      <c r="B2" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
+      <c r="D2" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
     </row>
     <row r="3" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>85</v>
+      <c r="B3" s="6" t="s">
+        <v>73</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="F3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
+      <c r="E3" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
     </row>
     <row r="4" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>86</v>
+      <c r="B4" s="6" t="s">
+        <v>74</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
+      <c r="D4" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
     </row>
     <row r="5" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>87</v>
+      <c r="B5" s="6" t="s">
+        <v>75</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
+      <c r="D5" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
     </row>
     <row r="6" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>88</v>
+      <c r="B6" s="6" t="s">
+        <v>76</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
+      <c r="D6" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
     </row>
     <row r="7" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>90</v>
+      <c r="A7" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>78</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
+      <c r="D7" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
     </row>
     <row r="8" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>92</v>
+      <c r="A8" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>80</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
+      <c r="D8" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
     </row>
     <row r="9" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>94</v>
+      <c r="A9" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>82</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
+      <c r="D9" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1495,73 +1480,90 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A12"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.1796875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="28.6328125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="21.08984375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="31.36328125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="18" style="5" customWidth="1"/>
+    <col min="6" max="6" width="18.90625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="19" style="5" customWidth="1"/>
+    <col min="8" max="8" width="10.90625" style="5" customWidth="1"/>
+    <col min="9" max="16384" width="8.7265625" style="5"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A9" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A10" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A11" s="5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A12" s="5" t="s">
-        <v>80</v>
-      </c>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="7" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" s="7" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add to cart tc
</commit_message>
<xml_diff>
--- a/LambdaTest_Playwright_Java/src/test/resources/TestCases/LambdaTest_Ecommerce Test Cases.xlsx
+++ b/LambdaTest_Playwright_Java/src/test/resources/TestCases/LambdaTest_Ecommerce Test Cases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="360" windowWidth="18820" windowHeight="7060" firstSheet="7" activeTab="8"/>
+    <workbookView xWindow="320" yWindow="360" windowWidth="18820" windowHeight="7060" firstSheet="7" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="TC01_Login" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,12 @@
     <sheet name="TC03_ForgotPassword" sheetId="2" r:id="rId3"/>
     <sheet name="TC05_MyAccount" sheetId="4" r:id="rId4"/>
     <sheet name="TC04_RegisterFromLoginPage" sheetId="5" r:id="rId5"/>
-    <sheet name="TC05_EditProfile" sheetId="6" r:id="rId6"/>
-    <sheet name="TC06_ChangePassword" sheetId="7" r:id="rId7"/>
-    <sheet name="TC07_AddAddress" sheetId="8" r:id="rId8"/>
-    <sheet name="TC08_EditDeleteAddress" sheetId="9" r:id="rId9"/>
-    <sheet name="TC09_AddToWishlist" sheetId="10" r:id="rId10"/>
-    <sheet name="TC10_AddToCart" sheetId="11" r:id="rId11"/>
+    <sheet name="TC06_EditProfile" sheetId="6" r:id="rId6"/>
+    <sheet name="TC07_ChangePassword" sheetId="7" r:id="rId7"/>
+    <sheet name="TC08_AddAddress" sheetId="8" r:id="rId8"/>
+    <sheet name="TC09_EditDeleteAddress" sheetId="9" r:id="rId9"/>
+    <sheet name="TC10_AddToWishlist" sheetId="10" r:id="rId10"/>
+    <sheet name="TC11_AddToCart" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -1426,8 +1426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2742,8 +2742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>